<commit_message>
l updated enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0D1137-676B-4359-A473-EE4697A69846}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9B205D-57E0-4C84-B685-30F9F1517528}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <t>paresh</t>
   </si>
   <si>
-    <t>paresh123</t>
+    <t>studyLanding</t>
   </si>
 </sst>
 </file>

</xml_diff>